<commit_message>
langchain and rag server incorporated
</commit_message>
<xml_diff>
--- a/agent_servers/output.xlsx
+++ b/agent_servers/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,33 +436,29 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>nombre</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>edad</t>
+          <t>Aqui tengo una mini tabla para que me la hagas excel:</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lucia</t>
+          <t>edad</t>
         </is>
-      </c>
-      <c r="B2" t="n">
-        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>25</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>33</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>